<commit_message>
Load and clean-up of post release defects
Load and clean-up of post release defects
</commit_message>
<xml_diff>
--- a/CA/JIRA/Plat Defects - Post Releases 7.6_7.7_7.8_8.0 cf v1-3 Found In Build Flag 280220.xlsx
+++ b/CA/JIRA/Plat Defects - Post Releases 7.6_7.7_7.8_8.0 cf v1-3 Found In Build Flag 280220.xlsx
@@ -20,13 +20,13 @@
   <calcPr calcId="145621"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId6"/>
-    <pivotCache cacheId="25" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId7"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7799" uniqueCount="1668">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7760" uniqueCount="1668">
   <si>
     <t>Issue Type</t>
   </si>
@@ -5529,7 +5529,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5556,12 +5556,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5803,8 +5797,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="244553984"/>
-        <c:axId val="244568448"/>
+        <c:axId val="448453248"/>
+        <c:axId val="448340736"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5981,11 +5975,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="244576256"/>
-        <c:axId val="244570368"/>
+        <c:axId val="448348544"/>
+        <c:axId val="448342656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="244553984"/>
+        <c:axId val="448453248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6013,7 +6007,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="244568448"/>
+        <c:crossAx val="448340736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6021,7 +6015,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244568448"/>
+        <c:axId val="448340736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6055,12 +6049,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="244553984"/>
+        <c:crossAx val="448453248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="244570368"/>
+        <c:axId val="448342656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6070,12 +6064,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="244576256"/>
+        <c:crossAx val="448348544"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="244576256"/>
+        <c:axId val="448348544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6085,7 +6079,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="244570368"/>
+        <c:crossAx val="448342656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7060,11 +7054,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="245222784"/>
-        <c:axId val="245232768"/>
+        <c:axId val="448884736"/>
+        <c:axId val="448886272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="245222784"/>
+        <c:axId val="448884736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7073,7 +7067,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="245232768"/>
+        <c:crossAx val="448886272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7081,7 +7075,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="245232768"/>
+        <c:axId val="448886272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7092,7 +7086,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="245222784"/>
+        <c:crossAx val="448884736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7139,7 +7133,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7240,8 +7233,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="244993408"/>
-        <c:axId val="244999680"/>
+        <c:axId val="448925696"/>
+        <c:axId val="448927616"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -7323,25 +7316,24 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="244993408"/>
-        <c:axId val="244999680"/>
+        <c:axId val="448925696"/>
+        <c:axId val="448927616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="244993408"/>
+        <c:axId val="448925696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="244999680"/>
+        <c:crossAx val="448927616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7349,7 +7341,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244999680"/>
+        <c:axId val="448927616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7357,21 +7349,19 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="244993408"/>
+        <c:crossAx val="448925696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -24288,8 +24278,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="AB3:AC61" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="AB3:AC17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="26">
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
@@ -24754,12 +24744,12 @@
         <item sd="0" x="2"/>
         <item sd="0" x="3"/>
         <item sd="0" x="6"/>
-        <item x="1"/>
+        <item sd="0" x="1"/>
         <item sd="0" x="5"/>
-        <item x="0"/>
-        <item x="7"/>
+        <item sd="0" x="0"/>
+        <item sd="0" x="7"/>
         <item sd="0" m="1" x="13"/>
-        <item x="9"/>
+        <item sd="0" x="9"/>
       </items>
     </pivotField>
   </pivotFields>
@@ -24768,7 +24758,7 @@
     <field x="19"/>
     <field x="23"/>
   </rowFields>
-  <rowItems count="58">
+  <rowItems count="14">
     <i>
       <x/>
     </i>
@@ -24796,149 +24786,17 @@
     <i>
       <x v="8"/>
     </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="9"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="11"/>
-    </i>
-    <i r="1">
-      <x v="12"/>
-    </i>
-    <i r="1">
-      <x v="13"/>
-    </i>
-    <i r="2">
-      <x v="9"/>
-    </i>
-    <i r="2">
-      <x v="229"/>
-    </i>
     <i>
       <x v="9"/>
     </i>
     <i>
       <x v="10"/>
     </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="9"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="11"/>
-    </i>
-    <i r="1">
-      <x v="12"/>
-    </i>
-    <i r="1">
-      <x v="13"/>
-    </i>
-    <i r="2">
-      <x v="103"/>
-    </i>
     <i>
       <x v="11"/>
     </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="9"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="12"/>
-    </i>
-    <i r="1">
-      <x v="13"/>
-    </i>
-    <i r="2">
-      <x v="179"/>
-    </i>
     <i>
       <x v="13"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
-    <i r="1">
-      <x v="9"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="12"/>
-    </i>
-    <i r="1">
-      <x v="13"/>
-    </i>
-    <i r="2">
-      <x v="231"/>
     </i>
     <i t="grand">
       <x/>
@@ -42676,8 +42534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X10" workbookViewId="0">
-      <selection activeCell="AB12" sqref="AB12"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AD25" sqref="AD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42699,7 +42557,7 @@
     <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="24.6640625" customWidth="1"/>
+    <col min="28" max="28" width="12.5546875" customWidth="1"/>
     <col min="29" max="29" width="17.77734375" customWidth="1"/>
     <col min="30" max="30" width="17" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="16" customWidth="1"/>
@@ -43331,7 +43189,9 @@
       <c r="AB12" s="5" t="s">
         <v>1657</v>
       </c>
-      <c r="AC12" s="6"/>
+      <c r="AC12" s="6">
+        <v>28</v>
+      </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -43377,11 +43237,11 @@
         <f t="shared" si="0"/>
         <v>7.6</v>
       </c>
-      <c r="AB13" s="14" t="s">
-        <v>86</v>
+      <c r="AB13" s="5" t="s">
+        <v>1658</v>
       </c>
       <c r="AC13" s="6">
-        <v>8</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.3">
@@ -43425,11 +43285,11 @@
         <f t="shared" si="0"/>
         <v>7.6</v>
       </c>
-      <c r="AB14" s="14" t="s">
-        <v>66</v>
+      <c r="AB14" s="5" t="s">
+        <v>1659</v>
       </c>
       <c r="AC14" s="6">
-        <v>4</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.3">
@@ -43473,11 +43333,11 @@
         <f t="shared" si="0"/>
         <v>7.7</v>
       </c>
-      <c r="AB15" s="14" t="s">
-        <v>1313</v>
+      <c r="AB15" s="5" t="s">
+        <v>1660</v>
       </c>
       <c r="AC15" s="6">
-        <v>1</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.3">
@@ -43524,11 +43384,11 @@
         <f t="shared" si="0"/>
         <v>7.7</v>
       </c>
-      <c r="AB16" s="14" t="s">
-        <v>82</v>
+      <c r="AB16" s="5" t="s">
+        <v>1664</v>
       </c>
       <c r="AC16" s="6">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.3">
@@ -43572,11 +43432,11 @@
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="AB17" s="14" t="s">
-        <v>74</v>
+      <c r="AB17" s="5" t="s">
+        <v>1343</v>
       </c>
       <c r="AC17" s="6">
-        <v>2</v>
+        <v>314</v>
       </c>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.3">
@@ -43620,12 +43480,6 @@
         <f t="shared" si="0"/>
         <v>7.2</v>
       </c>
-      <c r="AB18" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC18" s="6">
-        <v>2</v>
-      </c>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -43668,12 +43522,6 @@
         <f t="shared" si="0"/>
         <v>7.1</v>
       </c>
-      <c r="AB19" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC19" s="6">
-        <v>1</v>
-      </c>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -43716,12 +43564,6 @@
         <f t="shared" si="0"/>
         <v>8.0</v>
       </c>
-      <c r="AB20" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC20" s="6">
-        <v>6</v>
-      </c>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -43764,12 +43606,6 @@
         <f t="shared" si="0"/>
         <v>8.0</v>
       </c>
-      <c r="AB21" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC21" s="6">
-        <v>2</v>
-      </c>
       <c r="AE21" s="7" t="s">
         <v>1345</v>
       </c>
@@ -43821,12 +43657,6 @@
         <f t="shared" si="0"/>
         <v>7.4</v>
       </c>
-      <c r="AB22" s="15">
-        <v>43151.393750000003</v>
-      </c>
-      <c r="AC22" s="6">
-        <v>1</v>
-      </c>
       <c r="AE22" s="5">
         <v>7.5</v>
       </c>
@@ -43881,12 +43711,6 @@
         <f t="shared" si="0"/>
         <v>7.4</v>
       </c>
-      <c r="AB23" s="15">
-        <v>43696.527777777781</v>
-      </c>
-      <c r="AC23" s="6">
-        <v>1</v>
-      </c>
       <c r="AE23" s="5">
         <v>7.6</v>
       </c>
@@ -43941,12 +43765,6 @@
         <f t="shared" si="0"/>
         <v>7.6</v>
       </c>
-      <c r="AB24" s="5" t="s">
-        <v>1658</v>
-      </c>
-      <c r="AC24" s="6">
-        <v>49</v>
-      </c>
       <c r="AE24" s="5">
         <v>7.7</v>
       </c>
@@ -43998,10 +43816,6 @@
         <f t="shared" si="0"/>
         <v>8.0</v>
       </c>
-      <c r="AB25" s="5" t="s">
-        <v>1659</v>
-      </c>
-      <c r="AC25" s="6"/>
       <c r="AE25" s="12">
         <v>8</v>
       </c>
@@ -44053,12 +43867,6 @@
         <f t="shared" si="0"/>
         <v>7.6</v>
       </c>
-      <c r="AB26" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="AC26" s="6">
-        <v>6</v>
-      </c>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -44101,12 +43909,6 @@
         <f t="shared" si="0"/>
         <v>7.6</v>
       </c>
-      <c r="AB27" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC27" s="6">
-        <v>16</v>
-      </c>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -44149,12 +43951,6 @@
         <f t="shared" si="0"/>
         <v>7.6</v>
       </c>
-      <c r="AB28" s="14" t="s">
-        <v>1313</v>
-      </c>
-      <c r="AC28" s="6">
-        <v>6</v>
-      </c>
       <c r="AE28" t="s">
         <v>1665</v>
       </c>
@@ -44203,12 +43999,6 @@
         <f t="shared" si="0"/>
         <v>7.6</v>
       </c>
-      <c r="AB29" s="14" t="s">
-        <v>296</v>
-      </c>
-      <c r="AC29" s="6">
-        <v>4</v>
-      </c>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -44251,12 +44041,6 @@
         <f t="shared" si="0"/>
         <v>7.6</v>
       </c>
-      <c r="AB30" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="AC30" s="6">
-        <v>3</v>
-      </c>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -44302,12 +44086,6 @@
         <f t="shared" si="0"/>
         <v>8.0</v>
       </c>
-      <c r="AB31" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="AC31" s="6">
-        <v>5</v>
-      </c>
       <c r="AE31" t="s">
         <v>1345</v>
       </c>
@@ -44362,12 +44140,6 @@
         <f t="shared" si="0"/>
         <v>7.7</v>
       </c>
-      <c r="AB32" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="AC32" s="6">
-        <v>8</v>
-      </c>
       <c r="AE32">
         <v>7.5</v>
       </c>
@@ -44419,12 +44191,6 @@
         <f t="shared" si="0"/>
         <v>7.6</v>
       </c>
-      <c r="AB33" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC33" s="6">
-        <v>10</v>
-      </c>
       <c r="AE33">
         <v>7.6</v>
       </c>
@@ -44476,12 +44242,6 @@
         <f t="shared" si="0"/>
         <v>7.6</v>
       </c>
-      <c r="AB34" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC34" s="6">
-        <v>3</v>
-      </c>
       <c r="AE34">
         <v>7.7</v>
       </c>
@@ -44533,12 +44293,6 @@
         <f t="shared" si="0"/>
         <v>7.6</v>
       </c>
-      <c r="AB35" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC35" s="6">
-        <v>23</v>
-      </c>
       <c r="AE35" s="13">
         <v>8</v>
       </c>
@@ -44590,12 +44344,6 @@
         <f t="shared" si="0"/>
         <v>7.6</v>
       </c>
-      <c r="AB36" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC36" s="6">
-        <v>1</v>
-      </c>
     </row>
     <row r="37" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
@@ -44638,12 +44386,6 @@
         <f t="shared" si="0"/>
         <v>7.6</v>
       </c>
-      <c r="AB37" s="15">
-        <v>43497.178472222222</v>
-      </c>
-      <c r="AC37" s="6">
-        <v>1</v>
-      </c>
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
@@ -44692,10 +44434,6 @@
         <f t="shared" si="0"/>
         <v>7.7</v>
       </c>
-      <c r="AB38" s="5" t="s">
-        <v>1660</v>
-      </c>
-      <c r="AC38" s="6"/>
     </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -44738,12 +44476,6 @@
         <f t="shared" si="0"/>
         <v>7.2</v>
       </c>
-      <c r="AB39" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="AC39" s="6">
-        <v>5</v>
-      </c>
     </row>
     <row r="40" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
@@ -44786,12 +44518,6 @@
         <f t="shared" si="0"/>
         <v>7.2</v>
       </c>
-      <c r="AB40" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC40" s="6">
-        <v>8</v>
-      </c>
     </row>
     <row r="41" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
@@ -44840,12 +44566,6 @@
         <f t="shared" si="0"/>
         <v>7.6</v>
       </c>
-      <c r="AB41" s="14" t="s">
-        <v>1313</v>
-      </c>
-      <c r="AC41" s="6">
-        <v>2</v>
-      </c>
     </row>
     <row r="42" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
@@ -44888,12 +44608,6 @@
         <f t="shared" si="0"/>
         <v>8.0</v>
       </c>
-      <c r="AB42" s="14" t="s">
-        <v>296</v>
-      </c>
-      <c r="AC42" s="6">
-        <v>1</v>
-      </c>
     </row>
     <row r="43" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
@@ -44945,12 +44659,6 @@
         <f t="shared" si="0"/>
         <v>7.6</v>
       </c>
-      <c r="AB43" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="AC43" s="6">
-        <v>1</v>
-      </c>
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
@@ -44993,12 +44701,6 @@
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="AB44" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="AC44" s="6">
-        <v>2</v>
-      </c>
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
@@ -45041,12 +44743,6 @@
         <f t="shared" si="0"/>
         <v>7.6</v>
       </c>
-      <c r="AB45" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="AC45" s="6">
-        <v>3</v>
-      </c>
     </row>
     <row r="46" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
@@ -45089,12 +44785,6 @@
         <f t="shared" si="0"/>
         <v>8.0</v>
       </c>
-      <c r="AB46" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC46" s="6">
-        <v>2</v>
-      </c>
     </row>
     <row r="47" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
@@ -45137,12 +44827,6 @@
         <f t="shared" si="0"/>
         <v>8.0</v>
       </c>
-      <c r="AB47" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC47" s="6">
-        <v>18</v>
-      </c>
     </row>
     <row r="48" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
@@ -45185,14 +44869,8 @@
         <f t="shared" si="0"/>
         <v>7.0</v>
       </c>
-      <c r="AB48" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC48" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -45233,14 +44911,8 @@
         <f t="shared" si="0"/>
         <v>6.1</v>
       </c>
-      <c r="AB49" s="15">
-        <v>43605.65</v>
-      </c>
-      <c r="AC49" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -45281,12 +44953,8 @@
         <f t="shared" si="0"/>
         <v>8.0</v>
       </c>
-      <c r="AB50" s="5" t="s">
-        <v>1664</v>
-      </c>
-      <c r="AC50" s="6"/>
-    </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -45327,14 +44995,8 @@
         <f t="shared" si="0"/>
         <v>8.0</v>
       </c>
-      <c r="AB51" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC51" s="6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -45375,14 +45037,8 @@
         <f t="shared" si="0"/>
         <v>8.0</v>
       </c>
-      <c r="AB52" s="14" t="s">
-        <v>1313</v>
-      </c>
-      <c r="AC52" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -45426,14 +45082,8 @@
         <f t="shared" si="0"/>
         <v>7.6</v>
       </c>
-      <c r="AB53" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="AC53" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -45474,14 +45124,8 @@
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="AB54" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="AC54" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -45522,14 +45166,8 @@
         <f t="shared" si="0"/>
         <v>7.7</v>
       </c>
-      <c r="AB55" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="AC55" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -45573,14 +45211,8 @@
         <f t="shared" si="0"/>
         <v>7.6</v>
       </c>
-      <c r="AB56" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="AC56" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>10</v>
       </c>
@@ -45621,14 +45253,8 @@
         <f t="shared" si="0"/>
         <v>7.7</v>
       </c>
-      <c r="AB57" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC57" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>10</v>
       </c>
@@ -45666,14 +45292,8 @@
         <f t="shared" si="0"/>
         <v>8.0</v>
       </c>
-      <c r="AB58" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC58" s="6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>10</v>
       </c>
@@ -45714,14 +45334,8 @@
         <f t="shared" si="0"/>
         <v>7.6</v>
       </c>
-      <c r="AB59" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC59" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -45762,14 +45376,8 @@
         <f t="shared" si="0"/>
         <v>7.6</v>
       </c>
-      <c r="AB60" s="15">
-        <v>43696.691666666666</v>
-      </c>
-      <c r="AC60" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>10</v>
       </c>
@@ -45816,14 +45424,8 @@
         <f t="shared" si="0"/>
         <v>7.7</v>
       </c>
-      <c r="AB61" s="5" t="s">
-        <v>1343</v>
-      </c>
-      <c r="AC61" s="6">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -45868,7 +45470,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>10</v>
       </c>
@@ -45913,7 +45515,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>10</v>
       </c>

</xml_diff>